<commit_message>
update github link to pull request instead
</commit_message>
<xml_diff>
--- a/CS563-Project/Project/CS 563 Bug Mining.xlsx
+++ b/CS563-Project/Project/CS 563 Bug Mining.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\coding space\CS563-Project\CS563-Project\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5AA13ED-46B8-4418-8A6E-80FF5C0E2CE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBDB4CA2-153B-4692-80A7-F72724B3A5E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,75 +55,33 @@
     <t>ohsome</t>
   </si>
   <si>
-    <t>https://github.com/GIScience/ohsome-api/issues/10</t>
-  </si>
-  <si>
-    <t>https://github.com/GIScience/ohsome-api/issues/25</t>
-  </si>
-  <si>
-    <t>https://github.com/GIScience/ohsome-api/issues/26</t>
-  </si>
-  <si>
     <t>26/28</t>
   </si>
   <si>
-    <t>https://github.com/GIScience/ohsome-api/issues/59</t>
-  </si>
-  <si>
-    <t>https://github.com/GIScience/ohsome-api/issues/99</t>
-  </si>
-  <si>
-    <t>https://github.com/GIScience/ohsome-api/issues/109</t>
-  </si>
-  <si>
-    <t>https://github.com/GIScience/ohsome-api/issues/111</t>
-  </si>
-  <si>
-    <t>https://github.com/GIScience/ohsome-api/issues/129</t>
-  </si>
-  <si>
     <t>129/131</t>
   </si>
   <si>
-    <t>https://github.com/GIScience/ohsome-api/issues/141</t>
-  </si>
-  <si>
     <t>Missing/Null value</t>
   </si>
   <si>
-    <t>https://github.com/confluentinc/kafka-rest/issues/105</t>
-  </si>
-  <si>
     <t>Race condition exception</t>
   </si>
   <si>
     <t xml:space="preserve">kafka-rest </t>
   </si>
   <si>
-    <t>https://github.com/confluentinc/kafka-rest/issues/91</t>
-  </si>
-  <si>
     <t>Bad IdentityHashMap</t>
   </si>
   <si>
     <t>Custom paritioning not working</t>
   </si>
   <si>
-    <t>https://github.com/confluentinc/kafka-rest/issues/74</t>
-  </si>
-  <si>
-    <t>https://github.com/confluentinc/kafka-rest/issues/65</t>
-  </si>
-  <si>
     <t>Multiple consumer read requests with same ID hangs</t>
   </si>
   <si>
     <t>error when empty parameter</t>
   </si>
   <si>
-    <t>https://github.com/GIScience/ohsome-api/issues/2</t>
-  </si>
-  <si>
     <t>timeouts in data extraction request</t>
   </si>
   <si>
@@ -157,55 +115,97 @@
     <t>getMetadataTest sometimes fails</t>
   </si>
   <si>
-    <t>https://github.com/GIScience/ohsome-api/issues/175</t>
-  </si>
-  <si>
-    <t>https://github.com/GIScience/ohsome-api/issues/214</t>
-  </si>
-  <si>
     <t>Wrong error in case of  invalid coordinates</t>
   </si>
   <si>
-    <t>https://github.com/GIScience/ohsome-api/issues/289</t>
-  </si>
-  <si>
     <t>Internal Server Error when using changeset:… filter</t>
   </si>
   <si>
-    <t>https://github.com/GIScience/ohsome-api/issues/305</t>
-  </si>
-  <si>
     <t>changeset filter is not usable</t>
   </si>
   <si>
     <t>Unable to use a value containing a " " space</t>
   </si>
   <si>
-    <t>https://github.com/GIScience/ohsome-api/issues/313</t>
-  </si>
-  <si>
-    <t>https://github.com/GIScience/ohsome-api/issues/318</t>
-  </si>
-  <si>
     <t>Inconsistency in timestamps</t>
   </si>
   <si>
-    <t>https://github.com/fabioformosa/quartz-manager/issues/2</t>
-  </si>
-  <si>
     <t xml:space="preserve">quartz-manager </t>
   </si>
   <si>
     <t>Sometime have to re-create a new trigger</t>
   </si>
   <si>
-    <t>https://github.com/senzing-garage/senzing-api-server/issues/265</t>
-  </si>
-  <si>
     <t xml:space="preserve">senzing-api-server </t>
   </si>
   <si>
     <t>Spaces after a comma delimiter in CSV files causes incorrect parsing and incorrect data</t>
+  </si>
+  <si>
+    <t>https://github.com/GIScience/ohsome-api/pull/6</t>
+  </si>
+  <si>
+    <t>https://github.com/GIScience/oshdb/pull/258</t>
+  </si>
+  <si>
+    <t>https://github.com/GIScience/ohsome-api/pull/33</t>
+  </si>
+  <si>
+    <t>https://github.com/GIScience/ohsome-api/pull/27</t>
+  </si>
+  <si>
+    <t>https://github.com/GIScience/ohsome-api/pull/60</t>
+  </si>
+  <si>
+    <t>https://github.com/GIScience/ohsome-api/commit/c54cd1bedacefd0eac5674fff932fddd2e5c2232</t>
+  </si>
+  <si>
+    <t>https://github.com/GIScience/ohsome-api/pull/151</t>
+  </si>
+  <si>
+    <t>https://github.com/GIScience/ohsome-api/pull/112</t>
+  </si>
+  <si>
+    <t>https://github.com/GIScience/ohsome-api/pull/130</t>
+  </si>
+  <si>
+    <t>https://github.com/GIScience/ohsome-api/pull/144</t>
+  </si>
+  <si>
+    <t>https://github.com/GIScience/ohsome-api/commit/cda684d0aa7fb748ebe4205610f94b3961de4797</t>
+  </si>
+  <si>
+    <t>https://github.com/GIScience/ohsome-api/pull/215</t>
+  </si>
+  <si>
+    <t>https://github.com/GIScience/ohsome-api/pull/294</t>
+  </si>
+  <si>
+    <t>https://github.com/GIScience/ohsome-api/commit/44c01dccf285b2b1b494f0764f8f0f8bc987c362</t>
+  </si>
+  <si>
+    <t>https://github.com/GIScience/ohsome-api/pull/314</t>
+  </si>
+  <si>
+    <t>https://github.com/GIScience/ohsome-api/pull/319</t>
+  </si>
+  <si>
+    <t>https://github.com/confluentinc/kafka-rest/pull/144</t>
+  </si>
+  <si>
+    <t>https://github.com/confluentinc/kafka-rest/pull/222</t>
+  </si>
+  <si>
+    <t>https://github.com/confluentinc/kafka-rest/commit/e9c7bb73fb99519d4c38f824dd927687a6426466</t>
+  </si>
+  <si>
+    <t>https://github.com/confluentinc/kafka-rest/pull/67</t>
+  </si>
+  <si>
+    <t>https://github.com/fabioformosa/quartz-manager/commit/04da4556b14ca1d9f8a47406e6efc034a5e2ffd0</t>
+  </si>
+  <si>
+    <t>https://github.com/senzing-garage/senzing-api-server/pull/391/commits</t>
   </si>
 </sst>
 </file>
@@ -502,14 +502,14 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="14.42578125" customWidth="1"/>
     <col min="4" max="4" width="29.42578125" customWidth="1"/>
-    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="5" max="5" width="45" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -543,13 +543,13 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="F2" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -563,10 +563,10 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="F3" t="s">
         <v>6</v>
@@ -583,13 +583,13 @@
         <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="F4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -600,16 +600,16 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="E5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" t="s">
         <v>13</v>
-      </c>
-      <c r="F5" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -623,13 +623,13 @@
         <v>59</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="F6" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -643,10 +643,10 @@
         <v>99</v>
       </c>
       <c r="D7" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="F7" t="s">
         <v>9</v>
@@ -663,10 +663,10 @@
         <v>109</v>
       </c>
       <c r="D8" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="F8" t="s">
         <v>9</v>
@@ -683,10 +683,10 @@
         <v>111</v>
       </c>
       <c r="D9" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="F9" t="s">
         <v>8</v>
@@ -700,13 +700,13 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="F10" t="s">
         <v>9</v>
@@ -723,13 +723,13 @@
         <v>141</v>
       </c>
       <c r="D11" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="F11" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -743,10 +743,10 @@
         <v>175</v>
       </c>
       <c r="D12" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="F12" t="s">
         <v>7</v>
@@ -763,10 +763,10 @@
         <v>214</v>
       </c>
       <c r="D13" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="F13" t="s">
         <v>9</v>
@@ -783,10 +783,10 @@
         <v>289</v>
       </c>
       <c r="D14" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="F14" t="s">
         <v>9</v>
@@ -803,10 +803,10 @@
         <v>305</v>
       </c>
       <c r="D15" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="F15" t="s">
         <v>9</v>
@@ -823,10 +823,10 @@
         <v>313</v>
       </c>
       <c r="D16" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>8</v>
@@ -843,10 +843,10 @@
         <v>318</v>
       </c>
       <c r="D17" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>54</v>
       </c>
       <c r="F17" t="s">
         <v>9</v>
@@ -857,16 +857,16 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C18">
         <v>105</v>
       </c>
       <c r="D18" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="F18" t="s">
         <v>7</v>
@@ -877,16 +877,16 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C19">
         <v>91</v>
       </c>
       <c r="D19" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="F19" t="s">
         <v>7</v>
@@ -897,16 +897,16 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C20">
         <v>74</v>
       </c>
       <c r="D20" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="F20" t="s">
         <v>9</v>
@@ -917,16 +917,16 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C21">
         <v>65</v>
       </c>
       <c r="D21" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="F21" t="s">
         <v>7</v>
@@ -937,16 +937,16 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="C22">
         <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="F22" t="s">
         <v>7</v>
@@ -957,16 +957,16 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="C23">
         <v>265</v>
       </c>
       <c r="D23" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>59</v>
       </c>
       <c r="F23" t="s">
         <v>9</v>

</xml_diff>